<commit_message>
Matriz para usuarios MIR
</commit_message>
<xml_diff>
--- a/SIEDNL (PDR)/ENTREGABLES/Matriz de Pruebas/Matiz de Pruebas SIEDNL - MIR.xlsx
+++ b/SIEDNL (PDR)/ENTREGABLES/Matriz de Pruebas/Matiz de Pruebas SIEDNL - MIR.xlsx
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="143">
   <si>
     <t xml:space="preserve">Tester: Iris Lechuga </t>
   </si>
@@ -515,6 +515,33 @@
   </si>
   <si>
     <t xml:space="preserve">Cancela Registro </t>
+  </si>
+  <si>
+    <t>Configuración</t>
+  </si>
+  <si>
+    <t>Cambio de Contraseña</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cerrar serión </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inicio / Configiraciones </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muestra ventana principal de configuraciones </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modifica Cambio de Contraseña </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cierra Sesión </t>
+  </si>
+  <si>
+    <t>Cambia modificando la contraseña del usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cerrar Sesión </t>
   </si>
 </sst>
 </file>
@@ -1037,7 +1064,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1816,7 +1842,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -1948,7 +1973,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2246,7 +2270,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2367,7 +2390,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3127,7 +3149,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9729,128 +9750,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
-  <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="14">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="6"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Cuenta de N° Caso" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="5">
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="2">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="6" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="3">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="6" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="4">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="6" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="5">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="6" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica3" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A47:B49" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -10027,8 +9927,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="24">
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="24">
   <location ref="A24:B25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField dataField="1" showAll="0"/>
@@ -10096,9 +9996,130 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+  <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="14">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="6"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Cuenta de N° Caso" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="5">
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="5">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A6:N260" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" headerRowCellStyle="60% - Énfasis3">
-  <autoFilter ref="A6:N260"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A6:N263" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" headerRowCellStyle="60% - Énfasis3">
+  <autoFilter ref="A6:N263"/>
   <tableColumns count="14">
     <tableColumn id="1" name="N° Caso"/>
     <tableColumn id="2" name="Menús" dataDxfId="4"/>
@@ -10365,11 +10386,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:N283"/>
+  <dimension ref="A1:N286"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomLeft" activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -10544,7 +10565,7 @@
         <v>50</v>
       </c>
       <c r="G7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>51</v>
@@ -10700,10 +10721,10 @@
         <v>7</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>59</v>
+        <v>134</v>
       </c>
       <c r="D13" t="s">
         <v>86</v>
@@ -10712,13 +10733,13 @@
         <v>87</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>60</v>
+        <v>137</v>
       </c>
       <c r="G13" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>82</v>
+        <v>138</v>
       </c>
       <c r="N13" s="1"/>
     </row>
@@ -10727,10 +10748,10 @@
         <v>8</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>59</v>
+        <v>135</v>
       </c>
       <c r="D14" t="s">
         <v>86</v>
@@ -10739,25 +10760,25 @@
         <v>87</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>61</v>
+        <v>139</v>
       </c>
       <c r="G14" t="s">
         <v>16</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>22</v>
+        <v>141</v>
       </c>
       <c r="N14" s="1"/>
     </row>
-    <row r="15" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>9</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>59</v>
+        <v>136</v>
       </c>
       <c r="D15" t="s">
         <v>86</v>
@@ -10766,17 +10787,17 @@
         <v>87</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>62</v>
+        <v>140</v>
       </c>
       <c r="G15" t="s">
         <v>31</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>22</v>
+        <v>142</v>
       </c>
       <c r="N15" s="1"/>
     </row>
-    <row r="16" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="33" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>10</v>
       </c>
@@ -10793,28 +10814,25 @@
         <v>87</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="G16" t="s">
-        <v>31</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>109</v>
+        <v>33</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="N16" s="1"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" ht="33" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>11</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="D17" t="s">
         <v>86</v>
@@ -10823,29 +10841,25 @@
         <v>87</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G17" t="s">
-        <v>31</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>111</v>
+        <v>16</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="J17" s="3"/>
+        <v>22</v>
+      </c>
       <c r="N17" s="1"/>
     </row>
-    <row r="18" spans="1:14" ht="99" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="33" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>12</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="D18" t="s">
         <v>86</v>
@@ -10854,33 +10868,25 @@
         <v>87</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="G18" t="s">
-        <v>33</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="M18" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="N18" s="1">
-        <v>45083</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="66" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="N18" s="1"/>
+    </row>
+    <row r="19" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>13</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="D19" t="s">
         <v>86</v>
@@ -10889,20 +10895,20 @@
         <v>87</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G19" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="N19" s="1"/>
     </row>
-    <row r="20" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>14</v>
       </c>
@@ -10910,7 +10916,7 @@
         <v>59</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D20" t="s">
         <v>86</v>
@@ -10919,17 +10925,21 @@
         <v>87</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>112</v>
+        <v>64</v>
       </c>
       <c r="G20" t="s">
-        <v>16</v>
+        <v>31</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>113</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="J20" s="3"/>
       <c r="N20" s="1"/>
     </row>
-    <row r="21" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="99" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>15</v>
       </c>
@@ -10937,7 +10947,7 @@
         <v>59</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D21" t="s">
         <v>86</v>
@@ -10946,17 +10956,25 @@
         <v>87</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>112</v>
+        <v>73</v>
       </c>
       <c r="G21" t="s">
-        <v>16</v>
+        <v>33</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="N21" s="1"/>
-    </row>
-    <row r="22" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="M21" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="N21" s="1">
+        <v>45083</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="66" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>16</v>
       </c>
@@ -10964,7 +10982,7 @@
         <v>59</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D22" t="s">
         <v>86</v>
@@ -10973,13 +10991,16 @@
         <v>87</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>112</v>
+        <v>79</v>
       </c>
       <c r="G22" t="s">
         <v>16</v>
       </c>
+      <c r="H22" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="I22" s="3" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
       <c r="N22" s="1"/>
     </row>
@@ -10991,7 +11012,7 @@
         <v>59</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D23" t="s">
         <v>86</v>
@@ -11010,7 +11031,7 @@
       </c>
       <c r="N23" s="1"/>
     </row>
-    <row r="24" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>18</v>
       </c>
@@ -11018,7 +11039,7 @@
         <v>59</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D24" t="s">
         <v>86</v>
@@ -11033,11 +11054,11 @@
         <v>16</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="N24" s="1"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>19</v>
       </c>
@@ -11045,7 +11066,7 @@
         <v>59</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D25" t="s">
         <v>86</v>
@@ -11054,17 +11075,17 @@
         <v>87</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>70</v>
+        <v>112</v>
       </c>
       <c r="G25" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="N25" s="1"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>20</v>
       </c>
@@ -11072,7 +11093,7 @@
         <v>59</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D26" t="s">
         <v>86</v>
@@ -11080,14 +11101,14 @@
       <c r="E26" t="s">
         <v>87</v>
       </c>
-      <c r="F26" t="s">
-        <v>84</v>
+      <c r="F26" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="G26" t="s">
         <v>16</v>
       </c>
-      <c r="I26" t="s">
-        <v>85</v>
+      <c r="I26" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="N26" s="1"/>
     </row>
@@ -11107,14 +11128,14 @@
       <c r="E27" t="s">
         <v>87</v>
       </c>
-      <c r="F27" t="s">
-        <v>72</v>
+      <c r="F27" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="G27" t="s">
         <v>16</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="N27" s="1"/>
     </row>
@@ -11134,17 +11155,15 @@
       <c r="E28" t="s">
         <v>87</v>
       </c>
-      <c r="F28" t="s">
-        <v>89</v>
+      <c r="F28" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="G28" t="s">
-        <v>16</v>
-      </c>
-      <c r="H28"/>
+        <v>31</v>
+      </c>
       <c r="I28" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="J28"/>
+        <v>83</v>
+      </c>
       <c r="N28" s="1"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
@@ -11164,21 +11183,17 @@
         <v>87</v>
       </c>
       <c r="F29" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="G29" t="s">
-        <v>31</v>
-      </c>
-      <c r="H29" t="s">
-        <v>117</v>
+        <v>16</v>
       </c>
       <c r="I29" t="s">
-        <v>115</v>
-      </c>
-      <c r="J29"/>
+        <v>85</v>
+      </c>
       <c r="N29" s="1"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="33" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>24</v>
       </c>
@@ -11194,21 +11209,18 @@
       <c r="E30" t="s">
         <v>87</v>
       </c>
-      <c r="F30" s="3" t="s">
-        <v>91</v>
+      <c r="F30" t="s">
+        <v>72</v>
       </c>
       <c r="G30" t="s">
-        <v>31</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>116</v>
+        <v>16</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="N30" s="1"/>
     </row>
-    <row r="31" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>25</v>
       </c>
@@ -11224,90 +11236,117 @@
       <c r="E31" t="s">
         <v>87</v>
       </c>
-      <c r="F31" s="3" t="s">
-        <v>92</v>
+      <c r="F31" t="s">
+        <v>89</v>
       </c>
       <c r="G31" t="s">
-        <v>31</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>119</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="H31"/>
       <c r="I31" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="M31" t="s">
-        <v>42</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="J31"/>
       <c r="N31" s="1"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>26</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C32" t="s">
-        <v>93</v>
+      <c r="C32" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="D32" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E32" t="s">
-        <v>95</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>82</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="F32" t="s">
+        <v>90</v>
+      </c>
+      <c r="G32" t="s">
+        <v>31</v>
+      </c>
+      <c r="H32" t="s">
+        <v>117</v>
+      </c>
+      <c r="I32" t="s">
+        <v>115</v>
+      </c>
+      <c r="J32"/>
       <c r="N32" s="1"/>
     </row>
-    <row r="33" spans="2:14" ht="33" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>27</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C33" t="s">
-        <v>93</v>
+      <c r="C33" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="D33" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E33" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>62</v>
+        <v>91</v>
+      </c>
+      <c r="G33" t="s">
+        <v>31</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
       <c r="N33" s="1"/>
     </row>
-    <row r="34" spans="2:14" ht="33" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
+    <row r="34" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>28</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C34" t="s">
-        <v>93</v>
+      <c r="C34" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="D34" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E34" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
+      </c>
+      <c r="G34" t="s">
+        <v>31</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>22</v>
+        <v>118</v>
+      </c>
+      <c r="M34" t="s">
+        <v>42</v>
       </c>
       <c r="N34" s="1"/>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>29</v>
+      </c>
       <c r="B35" t="s">
         <v>59</v>
       </c>
@@ -11321,14 +11360,17 @@
         <v>95</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="N35" s="1"/>
     </row>
-    <row r="36" spans="2:14" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>30</v>
+      </c>
       <c r="B36" t="s">
         <v>59</v>
       </c>
@@ -11342,14 +11384,17 @@
         <v>95</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>98</v>
+        <v>62</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>123</v>
+        <v>22</v>
       </c>
       <c r="N36" s="1"/>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>31</v>
+      </c>
       <c r="B37" t="s">
         <v>59</v>
       </c>
@@ -11363,19 +11408,22 @@
         <v>95</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>124</v>
+        <v>22</v>
       </c>
       <c r="N37" s="1"/>
     </row>
-    <row r="38" spans="2:14" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>32</v>
+      </c>
       <c r="B38" t="s">
         <v>59</v>
       </c>
       <c r="C38" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="D38" t="s">
         <v>94</v>
@@ -11384,19 +11432,22 @@
         <v>95</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="N38" s="1"/>
     </row>
-    <row r="39" spans="2:14" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>33</v>
+      </c>
       <c r="B39" t="s">
         <v>59</v>
       </c>
       <c r="C39" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="D39" t="s">
         <v>94</v>
@@ -11405,19 +11456,22 @@
         <v>95</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="N39" s="1"/>
     </row>
-    <row r="40" spans="2:14" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>34</v>
+      </c>
       <c r="B40" t="s">
         <v>59</v>
       </c>
       <c r="C40" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
       <c r="D40" t="s">
         <v>94</v>
@@ -11426,19 +11480,22 @@
         <v>95</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="N40" s="1"/>
     </row>
-    <row r="41" spans="2:14" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>35</v>
+      </c>
       <c r="B41" t="s">
         <v>59</v>
       </c>
       <c r="C41" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D41" t="s">
         <v>94</v>
@@ -11447,19 +11504,22 @@
         <v>95</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="N41" s="1"/>
     </row>
-    <row r="42" spans="2:14" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>36</v>
+      </c>
       <c r="B42" t="s">
         <v>59</v>
       </c>
       <c r="C42" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D42" t="s">
         <v>94</v>
@@ -11475,12 +11535,15 @@
       </c>
       <c r="N42" s="1"/>
     </row>
-    <row r="43" spans="2:14" ht="33" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>37</v>
+      </c>
       <c r="B43" t="s">
         <v>59</v>
       </c>
       <c r="C43" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D43" t="s">
         <v>94</v>
@@ -11492,16 +11555,19 @@
         <v>112</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="N43" s="1"/>
     </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>38</v>
+      </c>
       <c r="B44" t="s">
         <v>59</v>
       </c>
       <c r="C44" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D44" t="s">
         <v>94</v>
@@ -11510,19 +11576,22 @@
         <v>95</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="N44" s="1"/>
     </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>39</v>
+      </c>
       <c r="B45" t="s">
         <v>59</v>
       </c>
       <c r="C45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D45" t="s">
         <v>94</v>
@@ -11531,14 +11600,17 @@
         <v>95</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>71</v>
+        <v>112</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>71</v>
+        <v>113</v>
       </c>
       <c r="N45" s="1"/>
     </row>
-    <row r="46" spans="2:14" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>40</v>
+      </c>
       <c r="B46" t="s">
         <v>59</v>
       </c>
@@ -11552,14 +11624,17 @@
         <v>95</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="N46" s="1"/>
     </row>
-    <row r="47" spans="2:14" ht="33" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>41</v>
+      </c>
       <c r="B47" t="s">
         <v>59</v>
       </c>
@@ -11573,14 +11648,17 @@
         <v>95</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
       <c r="N47" s="1"/>
     </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>42</v>
+      </c>
       <c r="B48" t="s">
         <v>59</v>
       </c>
@@ -11593,14 +11671,18 @@
       <c r="E48" t="s">
         <v>95</v>
       </c>
-      <c r="F48" t="s">
-        <v>89</v>
+      <c r="F48" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+      <c r="N48" s="1"/>
+    </row>
+    <row r="49" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>43</v>
+      </c>
       <c r="B49" t="s">
         <v>59</v>
       </c>
@@ -11613,14 +11695,18 @@
       <c r="E49" t="s">
         <v>95</v>
       </c>
-      <c r="F49" t="s">
-        <v>90</v>
+      <c r="F49" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+      <c r="N49" s="1"/>
+    </row>
+    <row r="50" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>44</v>
+      </c>
       <c r="B50" t="s">
         <v>59</v>
       </c>
@@ -11634,14 +11720,17 @@
         <v>95</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="N50" s="1"/>
     </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>45</v>
+      </c>
       <c r="B51" t="s">
         <v>59</v>
       </c>
@@ -11654,78 +11743,88 @@
       <c r="E51" t="s">
         <v>95</v>
       </c>
-      <c r="F51" s="3" t="s">
-        <v>92</v>
+      <c r="F51" t="s">
+        <v>89</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="N51" s="1"/>
-    </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>46</v>
+      </c>
       <c r="B52" t="s">
         <v>59</v>
       </c>
       <c r="C52" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="D52" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="E52" t="s">
-        <v>104</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
+      </c>
+      <c r="F52" t="s">
+        <v>90</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="N52" s="1"/>
-    </row>
-    <row r="53" spans="2:14" ht="33" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>47</v>
+      </c>
       <c r="B53" t="s">
         <v>59</v>
       </c>
       <c r="C53" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="D53" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="E53" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>22</v>
+        <v>120</v>
       </c>
       <c r="N53" s="1"/>
     </row>
-    <row r="54" spans="2:14" ht="33" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>48</v>
+      </c>
       <c r="B54" t="s">
         <v>59</v>
       </c>
       <c r="C54" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="D54" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="E54" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>22</v>
+        <v>128</v>
       </c>
       <c r="N54" s="1"/>
     </row>
-    <row r="55" spans="2:14" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>49</v>
+      </c>
       <c r="B55" t="s">
         <v>59</v>
       </c>
@@ -11739,14 +11838,17 @@
         <v>104</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="N55" s="1"/>
     </row>
-    <row r="56" spans="2:14" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>50</v>
+      </c>
       <c r="B56" t="s">
         <v>59</v>
       </c>
@@ -11760,14 +11862,17 @@
         <v>104</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>98</v>
+        <v>62</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>123</v>
+        <v>22</v>
       </c>
       <c r="N56" s="1"/>
     </row>
-    <row r="57" spans="2:14" ht="33" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>51</v>
+      </c>
       <c r="B57" t="s">
         <v>59</v>
       </c>
@@ -11781,14 +11886,17 @@
         <v>104</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>130</v>
+        <v>22</v>
       </c>
       <c r="N57" s="1"/>
     </row>
-    <row r="58" spans="2:14" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>52</v>
+      </c>
       <c r="B58" t="s">
         <v>59</v>
       </c>
@@ -11802,19 +11910,22 @@
         <v>104</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="N58" s="1"/>
     </row>
-    <row r="59" spans="2:14" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>53</v>
+      </c>
       <c r="B59" t="s">
         <v>59</v>
       </c>
       <c r="C59" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="D59" t="s">
         <v>103</v>
@@ -11823,19 +11934,22 @@
         <v>104</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="N59" s="1"/>
     </row>
-    <row r="60" spans="2:14" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>54</v>
+      </c>
       <c r="B60" t="s">
         <v>59</v>
       </c>
       <c r="C60" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="D60" t="s">
         <v>103</v>
@@ -11844,19 +11958,22 @@
         <v>104</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>113</v>
+        <v>130</v>
       </c>
       <c r="N60" s="1"/>
     </row>
-    <row r="61" spans="2:14" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>55</v>
+      </c>
       <c r="B61" t="s">
         <v>59</v>
       </c>
       <c r="C61" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
       <c r="D61" t="s">
         <v>103</v>
@@ -11865,19 +11982,22 @@
         <v>104</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="N61" s="1"/>
     </row>
-    <row r="62" spans="2:14" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>56</v>
+      </c>
       <c r="B62" t="s">
         <v>59</v>
       </c>
       <c r="C62" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D62" t="s">
         <v>103</v>
@@ -11893,12 +12013,15 @@
       </c>
       <c r="N62" s="1"/>
     </row>
-    <row r="63" spans="2:14" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>57</v>
+      </c>
       <c r="B63" t="s">
         <v>59</v>
       </c>
       <c r="C63" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D63" t="s">
         <v>103</v>
@@ -11914,12 +12037,15 @@
       </c>
       <c r="N63" s="1"/>
     </row>
-    <row r="64" spans="2:14" ht="33" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>58</v>
+      </c>
       <c r="B64" t="s">
         <v>59</v>
       </c>
       <c r="C64" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D64" t="s">
         <v>103</v>
@@ -11931,16 +12057,19 @@
         <v>112</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="N64" s="1"/>
     </row>
-    <row r="65" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>59</v>
+      </c>
       <c r="B65" t="s">
         <v>59</v>
       </c>
       <c r="C65" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D65" t="s">
         <v>103</v>
@@ -11949,19 +12078,22 @@
         <v>104</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>70</v>
+        <v>112</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="N65" s="1"/>
     </row>
-    <row r="66" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>60</v>
+      </c>
       <c r="B66" t="s">
         <v>59</v>
       </c>
       <c r="C66" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D66" t="s">
         <v>103</v>
@@ -11970,14 +12102,17 @@
         <v>104</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="N66" s="1"/>
     </row>
-    <row r="67" spans="2:14" ht="33" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>61</v>
+      </c>
       <c r="B67" t="s">
         <v>59</v>
       </c>
@@ -11991,14 +12126,17 @@
         <v>104</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="N67" s="1"/>
     </row>
-    <row r="68" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>62</v>
+      </c>
       <c r="B68" t="s">
         <v>59</v>
       </c>
@@ -12011,15 +12149,18 @@
       <c r="E68" t="s">
         <v>104</v>
       </c>
-      <c r="F68" t="s">
-        <v>89</v>
+      <c r="F68" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>89</v>
+        <v>133</v>
       </c>
       <c r="N68" s="1"/>
     </row>
-    <row r="69" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>63</v>
+      </c>
       <c r="B69" t="s">
         <v>59</v>
       </c>
@@ -12032,15 +12173,18 @@
       <c r="E69" t="s">
         <v>104</v>
       </c>
-      <c r="F69" t="s">
-        <v>90</v>
+      <c r="F69" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
       <c r="N69" s="1"/>
     </row>
-    <row r="70" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>64</v>
+      </c>
       <c r="B70" t="s">
         <v>59</v>
       </c>
@@ -12054,14 +12198,17 @@
         <v>104</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="N70" s="1"/>
     </row>
-    <row r="71" spans="2:14" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>65</v>
+      </c>
       <c r="B71" t="s">
         <v>59</v>
       </c>
@@ -12074,20 +12221,23 @@
       <c r="E71" t="s">
         <v>104</v>
       </c>
-      <c r="F71" s="3" t="s">
-        <v>92</v>
+      <c r="F71" t="s">
+        <v>89</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="N71" s="1"/>
     </row>
-    <row r="72" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B72" s="3" t="s">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>66</v>
+      </c>
+      <c r="B72" t="s">
         <v>59</v>
       </c>
       <c r="C72" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="D72" t="s">
         <v>103</v>
@@ -12095,36 +12245,99 @@
       <c r="E72" t="s">
         <v>104</v>
       </c>
-      <c r="F72" s="3" t="s">
+      <c r="F72" t="s">
+        <v>90</v>
+      </c>
+      <c r="I72" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="N72" s="1"/>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>67</v>
+      </c>
+      <c r="B73" t="s">
+        <v>59</v>
+      </c>
+      <c r="C73" t="s">
+        <v>69</v>
+      </c>
+      <c r="D73" t="s">
+        <v>103</v>
+      </c>
+      <c r="E73" t="s">
+        <v>104</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I73" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="N73" s="1"/>
+    </row>
+    <row r="74" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>68</v>
+      </c>
+      <c r="B74" t="s">
+        <v>59</v>
+      </c>
+      <c r="C74" t="s">
+        <v>69</v>
+      </c>
+      <c r="D74" t="s">
+        <v>103</v>
+      </c>
+      <c r="E74" t="s">
+        <v>104</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I74" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="N74" s="1"/>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>69</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C75" t="s">
+        <v>93</v>
+      </c>
+      <c r="D75" t="s">
+        <v>103</v>
+      </c>
+      <c r="E75" t="s">
+        <v>104</v>
+      </c>
+      <c r="F75" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="I72" s="3" t="s">
+      <c r="I75" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="N72" s="1"/>
-    </row>
-    <row r="73" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="N73" s="1"/>
-    </row>
-    <row r="74" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="N74" s="1"/>
-    </row>
-    <row r="75" spans="2:14" x14ac:dyDescent="0.3">
       <c r="N75" s="1"/>
     </row>
-    <row r="76" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
       <c r="N76" s="1"/>
     </row>
-    <row r="77" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
       <c r="N77" s="1"/>
     </row>
-    <row r="78" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="N78" s="1"/>
     </row>
-    <row r="79" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
       <c r="N79" s="1"/>
     </row>
-    <row r="80" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
       <c r="N80" s="1"/>
     </row>
     <row r="81" spans="14:14" x14ac:dyDescent="0.3">
@@ -12319,101 +12532,101 @@
     <row r="144" spans="14:14" x14ac:dyDescent="0.3">
       <c r="N144" s="1"/>
     </row>
-    <row r="145" spans="10:14" x14ac:dyDescent="0.3">
+    <row r="145" spans="14:14" x14ac:dyDescent="0.3">
       <c r="N145" s="1"/>
     </row>
-    <row r="146" spans="10:14" x14ac:dyDescent="0.3">
+    <row r="146" spans="14:14" x14ac:dyDescent="0.3">
       <c r="N146" s="1"/>
     </row>
-    <row r="147" spans="10:14" x14ac:dyDescent="0.3">
+    <row r="147" spans="14:14" x14ac:dyDescent="0.3">
       <c r="N147" s="1"/>
     </row>
-    <row r="148" spans="10:14" x14ac:dyDescent="0.3">
+    <row r="148" spans="14:14" x14ac:dyDescent="0.3">
       <c r="N148" s="1"/>
     </row>
-    <row r="149" spans="10:14" x14ac:dyDescent="0.3">
+    <row r="149" spans="14:14" x14ac:dyDescent="0.3">
       <c r="N149" s="1"/>
     </row>
-    <row r="150" spans="10:14" x14ac:dyDescent="0.3">
+    <row r="150" spans="14:14" x14ac:dyDescent="0.3">
       <c r="N150" s="1"/>
     </row>
-    <row r="151" spans="10:14" x14ac:dyDescent="0.3">
+    <row r="151" spans="14:14" x14ac:dyDescent="0.3">
       <c r="N151" s="1"/>
     </row>
-    <row r="152" spans="10:14" x14ac:dyDescent="0.3">
+    <row r="152" spans="14:14" x14ac:dyDescent="0.3">
       <c r="N152" s="1"/>
     </row>
-    <row r="153" spans="10:14" x14ac:dyDescent="0.3">
+    <row r="153" spans="14:14" x14ac:dyDescent="0.3">
       <c r="N153" s="1"/>
     </row>
-    <row r="154" spans="10:14" x14ac:dyDescent="0.3">
+    <row r="154" spans="14:14" x14ac:dyDescent="0.3">
       <c r="N154" s="1"/>
     </row>
-    <row r="155" spans="10:14" x14ac:dyDescent="0.3">
+    <row r="155" spans="14:14" x14ac:dyDescent="0.3">
       <c r="N155" s="1"/>
     </row>
-    <row r="156" spans="10:14" x14ac:dyDescent="0.3">
+    <row r="156" spans="14:14" x14ac:dyDescent="0.3">
       <c r="N156" s="1"/>
     </row>
-    <row r="157" spans="10:14" x14ac:dyDescent="0.3">
+    <row r="157" spans="14:14" x14ac:dyDescent="0.3">
       <c r="N157" s="1"/>
     </row>
-    <row r="158" spans="10:14" x14ac:dyDescent="0.3">
+    <row r="158" spans="14:14" x14ac:dyDescent="0.3">
       <c r="N158" s="1"/>
     </row>
-    <row r="159" spans="10:14" x14ac:dyDescent="0.3">
+    <row r="159" spans="14:14" x14ac:dyDescent="0.3">
       <c r="N159" s="1"/>
     </row>
-    <row r="160" spans="10:14" x14ac:dyDescent="0.3">
-      <c r="J160" s="6"/>
+    <row r="160" spans="14:14" x14ac:dyDescent="0.3">
       <c r="N160" s="1"/>
     </row>
-    <row r="161" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="161" spans="10:14" x14ac:dyDescent="0.3">
       <c r="N161" s="1"/>
     </row>
-    <row r="162" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="162" spans="10:14" x14ac:dyDescent="0.3">
       <c r="N162" s="1"/>
     </row>
-    <row r="163" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="163" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J163" s="6"/>
       <c r="N163" s="1"/>
     </row>
-    <row r="164" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="164" spans="10:14" x14ac:dyDescent="0.3">
       <c r="N164" s="1"/>
     </row>
-    <row r="165" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="165" spans="10:14" x14ac:dyDescent="0.3">
       <c r="N165" s="1"/>
     </row>
-    <row r="166" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="166" spans="10:14" x14ac:dyDescent="0.3">
       <c r="N166" s="1"/>
     </row>
-    <row r="167" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="167" spans="10:14" x14ac:dyDescent="0.3">
       <c r="N167" s="1"/>
     </row>
-    <row r="168" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="168" spans="10:14" x14ac:dyDescent="0.3">
       <c r="N168" s="1"/>
     </row>
-    <row r="169" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="169" spans="10:14" x14ac:dyDescent="0.3">
       <c r="N169" s="1"/>
     </row>
-    <row r="170" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="170" spans="10:14" x14ac:dyDescent="0.3">
       <c r="N170" s="1"/>
     </row>
-    <row r="171" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="171" spans="10:14" x14ac:dyDescent="0.3">
       <c r="N171" s="1"/>
     </row>
-    <row r="172" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="172" spans="10:14" x14ac:dyDescent="0.3">
       <c r="N172" s="1"/>
     </row>
-    <row r="173" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="173" spans="10:14" x14ac:dyDescent="0.3">
       <c r="N173" s="1"/>
     </row>
-    <row r="174" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="174" spans="10:14" x14ac:dyDescent="0.3">
       <c r="N174" s="1"/>
     </row>
-    <row r="175" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="175" spans="10:14" x14ac:dyDescent="0.3">
       <c r="N175" s="1"/>
     </row>
-    <row r="176" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="176" spans="10:14" x14ac:dyDescent="0.3">
       <c r="N176" s="1"/>
     </row>
     <row r="177" spans="10:14" x14ac:dyDescent="0.3">
@@ -12426,15 +12639,12 @@
       <c r="N179" s="1"/>
     </row>
     <row r="180" spans="10:14" x14ac:dyDescent="0.3">
-      <c r="J180" s="6"/>
       <c r="N180" s="1"/>
     </row>
     <row r="181" spans="10:14" x14ac:dyDescent="0.3">
-      <c r="J181" s="6"/>
       <c r="N181" s="1"/>
     </row>
     <row r="182" spans="10:14" x14ac:dyDescent="0.3">
-      <c r="J182" s="6"/>
       <c r="N182" s="1"/>
     </row>
     <row r="183" spans="10:14" x14ac:dyDescent="0.3">
@@ -12446,15 +12656,15 @@
       <c r="N184" s="1"/>
     </row>
     <row r="185" spans="10:14" x14ac:dyDescent="0.3">
-      <c r="J185" s="7"/>
+      <c r="J185" s="6"/>
       <c r="N185" s="1"/>
     </row>
     <row r="186" spans="10:14" x14ac:dyDescent="0.3">
-      <c r="J186" s="7"/>
+      <c r="J186" s="6"/>
       <c r="N186" s="1"/>
     </row>
     <row r="187" spans="10:14" x14ac:dyDescent="0.3">
-      <c r="J187" s="7"/>
+      <c r="J187" s="6"/>
       <c r="N187" s="1"/>
     </row>
     <row r="188" spans="10:14" x14ac:dyDescent="0.3">
@@ -12486,12 +12696,15 @@
       <c r="N194" s="1"/>
     </row>
     <row r="195" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J195" s="7"/>
       <c r="N195" s="1"/>
     </row>
     <row r="196" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J196" s="7"/>
       <c r="N196" s="1"/>
     </row>
     <row r="197" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J197" s="7"/>
       <c r="N197" s="1"/>
     </row>
     <row r="198" spans="10:14" x14ac:dyDescent="0.3">
@@ -12558,15 +12771,12 @@
       <c r="N218" s="1"/>
     </row>
     <row r="219" spans="10:14" x14ac:dyDescent="0.3">
-      <c r="J219" s="7"/>
       <c r="N219" s="1"/>
     </row>
     <row r="220" spans="10:14" x14ac:dyDescent="0.3">
-      <c r="J220" s="7"/>
       <c r="N220" s="1"/>
     </row>
     <row r="221" spans="10:14" x14ac:dyDescent="0.3">
-      <c r="J221" s="7"/>
       <c r="N221" s="1"/>
     </row>
     <row r="222" spans="10:14" x14ac:dyDescent="0.3">
@@ -12610,7 +12820,7 @@
       <c r="N231" s="1"/>
     </row>
     <row r="232" spans="10:14" x14ac:dyDescent="0.3">
-      <c r="J232" s="6"/>
+      <c r="J232" s="7"/>
       <c r="N232" s="1"/>
     </row>
     <row r="233" spans="10:14" x14ac:dyDescent="0.3">
@@ -12622,7 +12832,7 @@
       <c r="N234" s="1"/>
     </row>
     <row r="235" spans="10:14" x14ac:dyDescent="0.3">
-      <c r="J235" s="7"/>
+      <c r="J235" s="6"/>
       <c r="N235" s="1"/>
     </row>
     <row r="236" spans="10:14" x14ac:dyDescent="0.3">
@@ -12658,12 +12868,15 @@
       <c r="N243" s="1"/>
     </row>
     <row r="244" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J244" s="7"/>
       <c r="N244" s="1"/>
     </row>
     <row r="245" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J245" s="7"/>
       <c r="N245" s="1"/>
     </row>
     <row r="246" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J246" s="7"/>
       <c r="N246" s="1"/>
     </row>
     <row r="247" spans="10:14" x14ac:dyDescent="0.3">
@@ -12699,14 +12912,14 @@
     <row r="257" spans="14:14" x14ac:dyDescent="0.3">
       <c r="N257" s="1"/>
     </row>
-    <row r="261" spans="14:14" x14ac:dyDescent="0.3">
-      <c r="N261" s="1"/>
-    </row>
-    <row r="262" spans="14:14" x14ac:dyDescent="0.3">
-      <c r="N262" s="1"/>
-    </row>
-    <row r="263" spans="14:14" x14ac:dyDescent="0.3">
-      <c r="N263" s="1"/>
+    <row r="258" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N258" s="1"/>
+    </row>
+    <row r="259" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N259" s="1"/>
+    </row>
+    <row r="260" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N260" s="1"/>
     </row>
     <row r="264" spans="14:14" x14ac:dyDescent="0.3">
       <c r="N264" s="1"/>
@@ -12717,15 +12930,15 @@
     <row r="266" spans="14:14" x14ac:dyDescent="0.3">
       <c r="N266" s="1"/>
     </row>
+    <row r="267" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N267" s="1"/>
+    </row>
+    <row r="268" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N268" s="1"/>
+    </row>
     <row r="269" spans="14:14" x14ac:dyDescent="0.3">
       <c r="N269" s="1"/>
     </row>
-    <row r="270" spans="14:14" x14ac:dyDescent="0.3">
-      <c r="N270" s="1"/>
-    </row>
-    <row r="271" spans="14:14" x14ac:dyDescent="0.3">
-      <c r="N271" s="1"/>
-    </row>
     <row r="272" spans="14:14" x14ac:dyDescent="0.3">
       <c r="N272" s="1"/>
     </row>
@@ -12757,12 +12970,21 @@
       <c r="N281" s="1"/>
     </row>
     <row r="282" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E282" t="s">
+      <c r="N282" s="1"/>
+    </row>
+    <row r="283" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="N283" s="1"/>
+    </row>
+    <row r="284" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="N284" s="1"/>
+    </row>
+    <row r="285" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E285" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="283" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E283" t="s">
+    <row r="286" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E286" t="s">
         <v>23</v>
       </c>
     </row>
@@ -12778,7 +13000,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C7" r:id="rId1"/>
-    <hyperlink ref="M18" r:id="rId2"/>
+    <hyperlink ref="M21" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -12792,19 +13014,19 @@
           <x14:formula1>
             <xm:f>Datos!$D$2:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>K30:K284 K7:K27</xm:sqref>
+          <xm:sqref>K33:K287 K7:K30</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Datos!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G30:G284 G7:G27</xm:sqref>
+          <xm:sqref>G33:G287 G7:G30</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Datos!$C$2:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>L7:L304</xm:sqref>
+          <xm:sqref>L7:L307</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>